<commit_message>
Matriz de riesgo, ajuste de casos de prueba y plan de calidad
</commit_message>
<xml_diff>
--- a/Plan calidad.xlsx
+++ b/Plan calidad.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10. SOFKAU\2. Programación\3. QA\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BC3134-CE74-4A3A-8EDA-D64767E4D37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B28DD3-2C29-42C1-8EBD-3D90A258AD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de pruebas" sheetId="1" r:id="rId1"/>
+    <sheet name="Q-gates" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,34 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{6541FC49-0EE7-4B65-ABB1-33C8A47EC0D3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAsHHoQxQ
+Usuario de Windows    (2022-02-17 13:20:11)
+Usuario de Windows:</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t xml:space="preserve">Area </t>
   </si>
@@ -90,15 +117,6 @@
   </si>
   <si>
     <t>Release</t>
-  </si>
-  <si>
-    <t>Se realizarán pruebas funcionales para verificar el flujo de compras por parte de un usario registrado en Alkosto.</t>
-  </si>
-  <si>
-    <t>Verificar forma de pago Tarjeta crédito o débito. -Verificar forma de pago Bóton Bancolombia. -Verificar Transferencia por PSE. - Verificar tarjeta alkosto. -Verificar crédito 20 minutos</t>
-  </si>
-  <si>
-    <t>Verificar la compra de un producto. -Verificar la compra de multiples productos -Verificar el medio de pago efectivo Efecty</t>
   </si>
   <si>
     <t>1. El usuario debe tener acceso a la página web.                                                                                                                                                                                                                                                                                2. El usuario debe estar registrado y con una sesión inciada dentro del portal de Alkosto.
@@ -139,12 +157,93 @@
   <si>
     <t>Verificación de servicio SOA convertir numeros a moneda o texto.</t>
   </si>
+  <si>
+    <t>Se realizarán pruebas funcionales para verificar el flujo de compras por parte de un usario que se encuentra registrado en Alkosto.</t>
+  </si>
+  <si>
+    <t>Verificar que la operación suma efectúa la suma de dos números enteros, verificar que la operación resta efectua la resta entre dos números enteros, verificar que la operación multiplicación efectua la multiplicación de dos números enteros, verificar que la operación división efectua la división de sos números enteros, verificar que no es posible dividir a un numero entero entre cero, verificar que las operaciones suma, resta, multiplicación y división se efectuan bajo constantes como A y B.</t>
+  </si>
+  <si>
+    <t>Verificar que la calculadora opera sumas con más de dos sumandos. Verificar que la calculadora opera multiplicaciónes con más de dos números. Verificar que la calculadora opera con operaciones combinadas.</t>
+  </si>
+  <si>
+    <t>Se realizarán pruebas funcionales para verificar  la conversión de numeros a moneda tipo dólar  y numero en texto.</t>
+  </si>
+  <si>
+    <t>Verificar  la conversión de numero a texto, verificar la conversión de un numero a moneda tipo dólar.</t>
+  </si>
+  <si>
+    <t>Se probará las peticiones SOAT del servicio por medio de pruebas funcionales, donde se verificará la respuesta la operatividad de dos numeros con las operaciones suma, resta, multiplicaciones  y divisiones.</t>
+  </si>
+  <si>
+    <t>Se probará las peticiones SOAT del servicio por medio de pruebas funcionales, donde se verificará la conversión de un valor numerico a moneda tipo  dólar y a valor numerico en texto.</t>
+  </si>
+  <si>
+    <t>Q-Gates</t>
+  </si>
+  <si>
+    <t>Casos diseñados vs casos ejecutados</t>
+  </si>
+  <si>
+    <t>Casos de prueba diseñados</t>
+  </si>
+  <si>
+    <t>Casos de prueba ejecutados</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Casos diseñados vs casos fallidos</t>
+  </si>
+  <si>
+    <t>Casos de prueba fallidos</t>
+  </si>
+  <si>
+    <t>Errores Funcionales sin resolver</t>
+  </si>
+  <si>
+    <t>Errores No Funcionales de Severidad Crítica/ alta sin resolver</t>
+  </si>
+  <si>
+    <t>Errores No Funcionales de severidad crítica</t>
+  </si>
+  <si>
+    <t>Errores No Funcionales de severidad Alta</t>
+  </si>
+  <si>
+    <t>Bugs abiertos</t>
+  </si>
+  <si>
+    <t>Número total de bugs</t>
+  </si>
+  <si>
+    <t>Número de bugs  sin resolver</t>
+  </si>
+  <si>
+    <t>Historias Técnicas</t>
+  </si>
+  <si>
+    <t>Existe un análisis de las historias técnicas</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Verificar forma de pago Tarjeta crédito o débito. -Verificar forma de pago Bóton Bancolombia. -Verificar Transferencia por PSE. - Verificar tarjeta alkosto. -Verificar crédito 20 minutos. Verificar button de garantía extendida dentro de la pasarela de carrito de compra. -Verificar funcionamiento de button para verificar datos de usuario. -Verificar funcionamiento de button para verificar  button de agregar dirección. -Verificar button cambiar metodo de envío</t>
+  </si>
+  <si>
+    <t>Verificar la compra de un producto. -Verificar la compra de multiples productos -Verificar el medio de pago efectivo Efecty. -Verificar la cantidad de productos del mismo tipo que permite comprar, Verificar metodo de envío. Verificar disponibilidad en tienda. -Verificar el button eliminar producto del carrito de compra. - Verificar button continuar comprando, - Verificar button editar carrito, -Verificar forma de pago por Bono</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,8 +292,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +350,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9CC2E5"/>
+        <bgColor rgb="FF9CC2E5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -243,42 +380,524 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDEEAF6"/>
+          <bgColor rgb="FFDEEAF6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FFD8D8D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="7"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Ejemplo Matriz de Riesgo-style" pivot="0" count="3" xr9:uid="{D5881C17-EEA9-4DFB-9DD7-206F7B07F0B7}">
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="secondRowStripe" dxfId="13"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FF000099"/>
@@ -308,7 +927,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -406,6 +1025,201 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2828925" cy="1162050"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image5.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F720BB0F-44E5-4BCB-827E-F5570F472BAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6867525" y="409575"/>
+          <a:ext cx="2828925" cy="1162050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2647950" cy="1171575"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="image7.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C228B322-CDB0-4039-B1A0-3A2A6792EEE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13087350" y="257175"/>
+          <a:ext cx="2647950" cy="1171575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2743200" cy="657225"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="image6.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE7D4E2D-327D-4F72-A14E-DA4B27924266}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13087350" y="1771650"/>
+          <a:ext cx="2743200" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2752725" cy="552450"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="image4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D32BEF86-EDED-4DB9-A4A3-2A71C94CC2EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10144125" y="1800225"/>
+          <a:ext cx="2752725" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2771775" cy="647700"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="image3.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A8F8675-A03A-4FE5-B4F4-0B01EE24881D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6886575" y="3038475"/>
+          <a:ext cx="2771775" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -677,11 +1491,11 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="102" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
@@ -697,129 +1511,156 @@
     <col min="13" max="13" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:13" ht="51.75" customHeight="1">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="51" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="191.25">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="L3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="229.5">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="76.5">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -830,4 +1671,293 @@
   <pageSetup paperSize="144" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6332F239-9364-4B05-9027-FED31A2A8373}">
+  <dimension ref="B1:E17"/>
+  <sheetViews>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="5" width="33.42578125" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:5">
+      <c r="B2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="22"/>
+      <c r="C5" s="23">
+        <v>100</v>
+      </c>
+      <c r="D5" s="23">
+        <v>95</v>
+      </c>
+      <c r="E5" s="24">
+        <f>D5/C5</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="22"/>
+      <c r="C7" s="23">
+        <v>100</v>
+      </c>
+      <c r="D7" s="23">
+        <v>30</v>
+      </c>
+      <c r="E7" s="24">
+        <f>D7/C7</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="22"/>
+      <c r="C9" s="28">
+        <v>20</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="29">
+        <f>C9</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="30">
+      <c r="B10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="22"/>
+      <c r="C11" s="23">
+        <v>1</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0</v>
+      </c>
+      <c r="E11" s="29">
+        <f>C11+D11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="22"/>
+      <c r="C13" s="23">
+        <v>50</v>
+      </c>
+      <c r="D13" s="23">
+        <v>30</v>
+      </c>
+      <c r="E13" s="24">
+        <f>D13/C13</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="26"/>
+      <c r="E14" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B15" s="30"/>
+      <c r="C15" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33" t="str">
+        <f>C15</f>
+        <v>SI</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B17" s="30"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThanOrEqual">
+      <formula>95%</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThanOrEqual">
+      <formula>79%</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="between">
+      <formula>80%</formula>
+      <formula>94%</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThanOrEqual">
+      <formula>0.14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThanOrEqual">
+      <formula>0.15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThanOrEqual">
+      <formula>0.19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="greaterThanOrEqual">
+      <formula>0.2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+      <formula>"SI"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C15" xr:uid="{D8481ED3-ED2D-43CE-A180-0663DC3F277F}">
+      <formula1>"SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>